<commit_message>
correcoes no nome do cabecalho
</commit_message>
<xml_diff>
--- a/modelo_importacao_alunos.xlsx
+++ b/modelo_importacao_alunos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86858CE1-C548-4279-867C-B7CF1D604CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB679F6-218A-4ED0-8826-6BF66D0C7455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18615" yWindow="975" windowWidth="15375" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <t>Gênero</t>
   </si>
   <si>
-    <t xml:space="preserve">Data </t>
+    <t xml:space="preserve">Data de Nascimento </t>
   </si>
 </sst>
 </file>
@@ -88,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,6 +98,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,7 +334,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -350,27 +356,29 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>

</xml_diff>

<commit_message>
trata melhor erros na insercao dos dados e espacos em brancos no csv
</commit_message>
<xml_diff>
--- a/modelo_importacao_alunos.xlsx
+++ b/modelo_importacao_alunos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB679F6-218A-4ED0-8826-6BF66D0C7455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855E34D3-CE11-4457-827E-7A8E27478210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18615" yWindow="975" windowWidth="15375" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17580" yWindow="2010" windowWidth="15375" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <t>Gênero</t>
   </si>
   <si>
-    <t xml:space="preserve">Data de Nascimento </t>
+    <t>Data de Nascimento</t>
   </si>
 </sst>
 </file>
@@ -334,7 +334,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>